<commit_message>
feat: convert site to PWA with manifest, icons and service worker
</commit_message>
<xml_diff>
--- a/a_vroters_members (1) — копия.xlsx
+++ b/a_vroters_members (1) — копия.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1111/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1111/brokeerleads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED47EDA-AECA-7143-B77C-DE3D6E162206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E55031-0C55-6944-8168-4BD869D6EAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="25600" windowHeight="15380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13520,8 +13520,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I1809"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="110" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113:D255"/>
+    <sheetView tabSelected="1" topLeftCell="A346" zoomScale="110" workbookViewId="0">
+      <selection activeCell="D354" sqref="D354:D375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>